<commit_message>
@williamjreid Adding review of Matts section, plus more results
Re-ran a set of results
</commit_message>
<xml_diff>
--- a/assignment2/trunk/Results/TestRun_Will/TTP.xlsx
+++ b/assignment2/trunk/Results/TestRun_Will/TTP.xlsx
@@ -382,7 +382,7 @@
   <dimension ref="A1:B231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N254" sqref="N254"/>
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -893,121 +893,122 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <v>1474573.6378413399</v>
+        <v>1478775.77</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106">
-        <v>1474457.41330805</v>
+        <v>1478767.14</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <v>1474612.9589529899</v>
+        <v>1478883.78</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108">
-        <v>1475014.7796726699</v>
+        <v>1478880.21</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <v>1475072.0080252299</v>
+        <v>1478884.21</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <v>1474700.92648507</v>
+        <v>1478831.29</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111">
-        <v>1474512.85887483</v>
+        <v>1478729.77</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112">
-        <v>1474131.37335991</v>
+        <v>1478735.34</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <v>1474661.3499920999</v>
+        <v>1478767.97</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>1474540.84831732</v>
+        <v>1478758.79</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>1474559.90940592</v>
+        <v>1478794.34</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>1475406.9689853501</v>
+        <v>1478759.13</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>1475197.10805699</v>
+        <v>1478859.29</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>1474376.9313905099</v>
+        <v>1478885.59</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <v>1474237.2362468899</v>
+        <v>1478875.44</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>1474393.23215211</v>
+        <v>1478821.34</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>1474885.44649635</v>
+        <v>1478800.44</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>1477566.3372621599</v>
+        <v>1478891.23</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <v>1477983.56075261</v>
+        <v>1478764.58</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>1474972.9479167501</v>
+        <v>1478760.86</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
         <f>AVERAGE(A105:A124)</f>
-        <v>1474992.8916747575</v>
+        <v>1478811.3254999998</v>
       </c>
       <c r="B126">
         <f>MAX(A105:A124)</f>
-        <v>1477983.56075261</v>
+        <v>1478891.23</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>12004.4334</v>
+        <f>6001.24055743+6001.27175</f>
+        <v>12002.512307429999</v>
       </c>
       <c r="B127">
         <f>A127/COUNT(A105:A124)</f>
-        <v>600.22167000000002</v>
+        <v>600.12561537149998</v>
       </c>
     </row>
     <row r="130" spans="1:1">

</xml_diff>

<commit_message>
@williamjreid Updated E5 from notes, added another results table
</commit_message>
<xml_diff>
--- a/assignment2/trunk/Results/TestRun_Will/TTP.xlsx
+++ b/assignment2/trunk/Results/TestRun_Will/TTP.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Exercise 2" sheetId="1" r:id="rId1"/>
+    <sheet name="Exercise 4" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>a280_279</t>
   </si>
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1514,12 +1514,213 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1667.1041398136299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>4127.2632729134702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3869.2032729134698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>1235.46984738984</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>231.27984738984699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>4688.2632729134702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>4205.8032729134702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>489.00413981362999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>388.35984738984899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>2462.83998930708</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <f>AVERAGE(A2:A11)</f>
+        <v>2336.4590902757759</v>
+      </c>
+      <c r="B13">
+        <f>MAX(A2:A11)</f>
+        <v>4688.2632729134702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>-264555.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>-257430.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>-261865.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>-272915.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>-260774.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>-248197.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>-254304.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>-264046.40000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>-263101.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>-262301.59999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <f>AVERAGE(A16:A25)</f>
+        <v>-260949.37999999998</v>
+      </c>
+      <c r="B27">
+        <f>MAX(A16:A25)</f>
+        <v>-248197.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>-731106.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>-747580.05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>-787200.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>-737779.14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>-736110.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>-722973.51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>-741949.74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>-712129.95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>-727978.23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>-714215.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <f>AVERAGE(A30:A39)</f>
+        <v>-735902.37000000011</v>
+      </c>
+      <c r="B41">
+        <f>MAX(A30:A39)</f>
+        <v>-712129.95</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
@williamjreid Minor checks and commenting updates
</commit_message>
<xml_diff>
--- a/assignment2/trunk/Results/TestRun_Will/TTP.xlsx
+++ b/assignment2/trunk/Results/TestRun_Will/TTP.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Exercise 2" sheetId="1" r:id="rId1"/>
-    <sheet name="Exercise 4" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Exercise 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Exercise 4" sheetId="2" r:id="rId3"/>
+    <sheet name="Exercise 4(2)" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>a280_279</t>
   </si>
@@ -1514,11 +1515,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1725,14 +1738,130 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>3473.92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>6164.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>5616.14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <f>AVERAGE(A2:A4)</f>
+        <v>5085.0099999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>-162238.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>-205335.97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <f>AVERAGE(A10:A11)</f>
+        <v>-183787.20500000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>-620626.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>-444818.84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <f>AVERAGE(A17:A18)</f>
+        <v>-532722.87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>-6927376.7699999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>-6926291.1500000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <f>AVERAGE(A24:A25)</f>
+        <v>-6926833.96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>-86880402.019999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31">
+        <v>-86539272.709999993</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <f>AVERAGE(A30:A31)</f>
+        <v>-86709837.364999995</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>